<commit_message>
Feat: refresh the pdf-weaver web
</commit_message>
<xml_diff>
--- a/documentation/marketing/CompareSimplePortfolio.xlsx
+++ b/documentation/marketing/CompareSimplePortfolio.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\greinke\cryptng\documentation\marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3145A381-33A0-4725-9D0F-C2BCC6991897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6721D30-E483-4B29-89B9-8091C02E9D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2242" yWindow="2242" windowWidth="19562" windowHeight="10161" xr2:uid="{EEB16ED2-DAE1-4CE4-9D23-039A6DA85D03}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{EEB16ED2-DAE1-4CE4-9D23-039A6DA85D03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>1 PDF</t>
   </si>
@@ -83,16 +84,76 @@
   </si>
   <si>
     <t>Pdf Weaver</t>
+  </si>
+  <si>
+    <t>Cost per h Energy</t>
+  </si>
+  <si>
+    <t>Parallel Pdf Pages per h</t>
+  </si>
+  <si>
+    <t>per year</t>
+  </si>
+  <si>
+    <t>Cost Energy per year</t>
+  </si>
+  <si>
+    <t>Seconds per page</t>
+  </si>
+  <si>
+    <t>Parallel Server</t>
+  </si>
+  <si>
+    <t>Load per h</t>
+  </si>
+  <si>
+    <t>max Pages</t>
+  </si>
+  <si>
+    <t>Executions</t>
+  </si>
+  <si>
+    <t>Packages per Year</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Cost per package</t>
+  </si>
+  <si>
+    <t>Cost per Customer</t>
+  </si>
+  <si>
+    <t>Cost per Year</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Bandwidth per Month</t>
+  </si>
+  <si>
+    <t>Bandwidth per Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,17 +179,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{568EEB60-6713-40A7-B98E-04EF09B94770}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="A1:F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -934,4 +1001,303 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5503D69C-0D5D-4692-A1B2-D334581ECAEC}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="19.25" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="18.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>0.4</f>
+        <v>0.4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f>60*60/B2*C2</f>
+        <v>2880</v>
+      </c>
+      <c r="F2" s="3">
+        <f>E2*24*365</f>
+        <v>25228800</v>
+      </c>
+      <c r="G2">
+        <f>A2*24*365</f>
+        <v>3504.0000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4">
+        <f>A4*B4*C4*D4/365/24</f>
+        <v>45.662100456621005</v>
+      </c>
+      <c r="F4" s="3">
+        <f>E4*24*365</f>
+        <v>400000</v>
+      </c>
+      <c r="G4" s="4">
+        <f>A4*B4/E2*A2</f>
+        <v>1.3888888888888891</v>
+      </c>
+      <c r="H4" s="4">
+        <f>G4*C4</f>
+        <v>5.5555555555555562</v>
+      </c>
+      <c r="I4" s="4">
+        <f>H4*D4</f>
+        <v>55.555555555555564</v>
+      </c>
+      <c r="J4">
+        <f>50*C4*D4</f>
+        <v>2000</v>
+      </c>
+      <c r="K4" s="5">
+        <f>0.1*3/1024*A4*C4*D4/12</f>
+        <v>0.97656250000000011</v>
+      </c>
+      <c r="L4" s="6">
+        <f>K4*12</f>
+        <v>11.718750000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>5000</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" ref="E5:E6" si="0">A5*B5*C5*D5/365/24</f>
+        <v>136.98630136986301</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F8" si="1">E5*24*365</f>
+        <v>1200000</v>
+      </c>
+      <c r="G5" s="4">
+        <f>A5*B5/E2*A2</f>
+        <v>6.9444444444444446</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5:I5" si="2">G5*C5</f>
+        <v>20.833333333333336</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="2"/>
+        <v>166.66666666666669</v>
+      </c>
+      <c r="J5">
+        <f>100*C5*D5</f>
+        <v>2400</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" ref="K5:K6" si="3">0.1*3/1024*A5*C5*D5/12</f>
+        <v>2.9296875000000004</v>
+      </c>
+      <c r="L5" s="6">
+        <f t="shared" ref="L5:L8" si="4">K5*12</f>
+        <v>35.156250000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>114.15525114155251</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="G6" s="4">
+        <f>A6*B6/E2*A2</f>
+        <v>13.888888888888889</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6:I6" si="5">G6*C6</f>
+        <v>27.777777777777779</v>
+      </c>
+      <c r="I6" s="4">
+        <f t="shared" si="5"/>
+        <v>138.88888888888889</v>
+      </c>
+      <c r="J6">
+        <f>200*C6*D6</f>
+        <v>2000</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="3"/>
+        <v>2.4414062500000004</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" si="4"/>
+        <v>29.296875000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>900000</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" ref="E7:E8" si="6">A8*B8*C8*D8/365/24</f>
+        <v>1027.3972602739725</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>9000000</v>
+      </c>
+      <c r="G8" s="4">
+        <f>A8*B8/E2*A2</f>
+        <v>1250</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" ref="H7:H8" si="7">G8*C8</f>
+        <v>1250</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" ref="I7:I8" si="8">H8*D8</f>
+        <v>1250</v>
+      </c>
+      <c r="J8">
+        <f>5000*C8*D8</f>
+        <v>5000</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" ref="K7:K8" si="9">0.1*3/1024*A8*C8*D8/12</f>
+        <v>21.972656250000004</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="4"/>
+        <v>263.67187500000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>